<commit_message>
updating srs and RTM
</commit_message>
<xml_diff>
--- a/Monitor and Control/Traceability Matrix.xlsx
+++ b/Monitor and Control/Traceability Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI Study\QA Project\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F709421E-FC8E-466B-8664-59FFF4F31081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E0FC28-AD4D-44A3-8E15-D29F8D246A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -583,21 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,9 +593,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,8 +610,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -904,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="C23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="A33:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -919,22 +925,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
@@ -943,10 +949,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="6" t="s">
         <v>73</v>
       </c>
@@ -957,22 +963,22 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="9" t="s">
         <v>128</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -981,148 +987,148 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="7" t="s">
         <v>111</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="12" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -1131,106 +1137,106 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="8" t="s">
         <v>108</v>
       </c>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="9" t="s">
         <v>124</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -1239,24 +1245,24 @@
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="7" t="s">
         <v>105</v>
       </c>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>122</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -1268,7 +1274,7 @@
       <c r="E22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="12" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="8" t="s">
@@ -1277,8 +1283,8 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="21"/>
       <c r="D23" s="8" t="s">
         <v>24</v>
@@ -1286,15 +1292,15 @@
       <c r="E23" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="8" t="s">
         <v>106</v>
       </c>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="21"/>
       <c r="D24" s="8" t="s">
         <v>25</v>
@@ -1302,29 +1308,29 @@
       <c r="E24" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="8" t="s">
         <v>106</v>
       </c>
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="12" t="s">
         <v>90</v>
       </c>
       <c r="G25" s="8" t="s">
@@ -1333,120 +1339,120 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="8" t="s">
         <v>110</v>
       </c>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
       <c r="G32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H32" s="8"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G33" s="7" t="s">
@@ -1454,149 +1460,149 @@
       </c>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
       <c r="G34" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
       <c r="G40" s="7" t="s">
         <v>115</v>
       </c>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
       <c r="G41" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
       <c r="G42" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="12" t="s">
         <v>93</v>
       </c>
       <c r="G43" s="8" t="s">
@@ -1604,163 +1610,163 @@
       </c>
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H44" s="8"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
       <c r="G46" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
       <c r="G47" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H48" s="8"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
       <c r="D49" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
       <c r="D50" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
       <c r="G50" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H50" s="8"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
       <c r="D52" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
       <c r="G52" s="8" t="s">
         <v>117</v>
       </c>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
       <c r="G53" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="9" t="s">
         <v>65</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="9" t="s">
         <v>92</v>
       </c>
       <c r="G54" s="7" t="s">
@@ -1769,84 +1775,84 @@
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
       <c r="G55" s="7" t="s">
         <v>119</v>
       </c>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="15"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
       <c r="D56" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
       <c r="G56" s="7" t="s">
         <v>119</v>
       </c>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
       <c r="G57" s="7" t="s">
         <v>119</v>
       </c>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
       <c r="G58" s="7" t="s">
         <v>119</v>
       </c>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
       <c r="G59" s="7" t="s">
         <v>120</v>
       </c>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
       <c r="G60" s="7" t="s">
         <v>119</v>
       </c>
@@ -2618,32 +2624,10 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="F54:F60"/>
-    <mergeCell ref="A43:A53"/>
-    <mergeCell ref="B43:B53"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:E12"/>
-    <mergeCell ref="E13:E19"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F13:F19"/>
-    <mergeCell ref="F3:F12"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="E33:E42"/>
-    <mergeCell ref="E54:E60"/>
-    <mergeCell ref="C54:C60"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="B33:B42"/>
-    <mergeCell ref="B54:B60"/>
-    <mergeCell ref="C33:C42"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="B13:B19"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E25:E32"/>
-    <mergeCell ref="F25:F32"/>
+    <mergeCell ref="E43:E53"/>
+    <mergeCell ref="F43:F53"/>
+    <mergeCell ref="C25:C32"/>
+    <mergeCell ref="F33:F42"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
@@ -2655,13 +2639,35 @@
     <mergeCell ref="C3:C12"/>
     <mergeCell ref="C13:C19"/>
     <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E25:E32"/>
+    <mergeCell ref="F25:F32"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="F22:F24"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:E12"/>
+    <mergeCell ref="E13:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F13:F19"/>
+    <mergeCell ref="F3:F12"/>
+    <mergeCell ref="F54:F60"/>
+    <mergeCell ref="A43:A53"/>
+    <mergeCell ref="B43:B53"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="E33:E42"/>
+    <mergeCell ref="E54:E60"/>
+    <mergeCell ref="C54:C60"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="B33:B42"/>
+    <mergeCell ref="B54:B60"/>
+    <mergeCell ref="C33:C42"/>
+    <mergeCell ref="A33:A42"/>
     <mergeCell ref="C43:C53"/>
-    <mergeCell ref="E43:E53"/>
-    <mergeCell ref="F43:F53"/>
-    <mergeCell ref="C25:C32"/>
-    <mergeCell ref="F33:F42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update RTM and PMP
</commit_message>
<xml_diff>
--- a/Monitor and Control/Traceability Matrix.xlsx
+++ b/Monitor and Control/Traceability Matrix.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\TravelAdvisor\Monitor and Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\TravelAdvisor\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB940C11-F01C-470A-9E0D-126089C57387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="173">
   <si>
     <t>Specific requirements</t>
   </si>
@@ -546,11 +547,53 @@
   <si>
     <t>TC_User_Home_003</t>
   </si>
+  <si>
+    <t>TC_AddTour_001
+TC_AddTour_002
+TC_AddTour_003
+TC_AddTour_004
+TC_AddTour_005</t>
+  </si>
+  <si>
+    <t>TC_AddTour_006
+TC_AddTour_007
+TC_AddTour_008
+TC_AddTour_009
+TC_AddTour_010
+TC_AddTour_011</t>
+  </si>
+  <si>
+    <t>TC_AddTour_012
+TC_AddTour_013
+TC_AddTour_014
+TC_AddTour_015
+TC_AddTour_016
+TC_AddTour_017
+TC_AddTour_018
+TC_AddTour_019
+TC_AddTour_020
+TC_AddTour_021</t>
+  </si>
+  <si>
+    <t>TC_AddTour_022</t>
+  </si>
+  <si>
+    <t>TC_AddTour_023
+TC_AddTour_024</t>
+  </si>
+  <si>
+    <t>TC_AddTour_025
+TC_AddTour_026</t>
+  </si>
+  <si>
+    <t>TC_Thank_You_001
+TC_Thank_You_002</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -726,16 +769,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,7 +793,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -756,29 +814,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,11 +1105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,22 +1123,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1101,10 +1147,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="6" t="s">
         <v>73</v>
       </c>
@@ -1115,22 +1161,22 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>128</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -1139,148 +1185,148 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="7" t="s">
         <v>96</v>
       </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="7" t="s">
         <v>111</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="16" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -1291,15 +1337,15 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="14" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="16" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="11" t="s">
@@ -1307,63 +1353,63 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="11" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="11" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="11" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="14" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="14" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="16" t="s">
         <v>97</v>
       </c>
       <c r="H19" s="11" t="s">
@@ -1371,26 +1417,26 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="15"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="11" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="8" t="s">
         <v>97</v>
       </c>
@@ -1399,14 +1445,14 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="8" t="s">
         <v>97</v>
       </c>
@@ -1415,14 +1461,14 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="11" t="s">
         <v>97</v>
       </c>
@@ -1431,15 +1477,15 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="14" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="14" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="16" t="s">
         <v>108</v>
       </c>
       <c r="H24" s="11" t="s">
@@ -1447,27 +1493,27 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="15"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="11" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="14" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="14" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="16" t="s">
         <v>97</v>
       </c>
       <c r="H26" s="13" t="s">
@@ -1475,26 +1521,26 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="15"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="11" t="s">
         <v>108</v>
       </c>
@@ -1503,14 +1549,14 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="15"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="11" t="s">
         <v>97</v>
       </c>
@@ -1519,40 +1565,40 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="15" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="7" t="s">
         <v>105</v>
       </c>
@@ -1561,13 +1607,13 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="16" t="s">
         <v>121</v>
       </c>
       <c r="B32" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="26" t="s">
         <v>123</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -1576,7 +1622,7 @@
       <c r="E32" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G32" s="8" t="s">
@@ -1585,54 +1631,56 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="17"/>
       <c r="G33" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="8"/>
+      <c r="H33" s="13" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="15"/>
+      <c r="F34" s="18"/>
       <c r="G34" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="8"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="16" t="s">
         <v>90</v>
       </c>
       <c r="G35" s="8" t="s">
@@ -1643,14 +1691,14 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="8" t="s">
         <v>97</v>
       </c>
@@ -1659,14 +1707,14 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
       <c r="G37" s="8" t="s">
         <v>97</v>
       </c>
@@ -1675,14 +1723,14 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
       <c r="G38" s="8" t="s">
         <v>97</v>
       </c>
@@ -1691,14 +1739,14 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
       <c r="D39" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
       <c r="G39" s="8" t="s">
         <v>97</v>
       </c>
@@ -1707,14 +1755,14 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="8" t="s">
         <v>110</v>
       </c>
@@ -1723,14 +1771,14 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
       <c r="G41" s="8" t="s">
         <v>97</v>
       </c>
@@ -1739,14 +1787,14 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
       <c r="G42" s="8" t="s">
         <v>97</v>
       </c>
@@ -1755,22 +1803,22 @@
       </c>
     </row>
     <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="18" t="s">
+      <c r="F43" s="19" t="s">
         <v>91</v>
       </c>
       <c r="G43" s="7" t="s">
@@ -1779,148 +1827,148 @@
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="19"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="19"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="19"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="20"/>
       <c r="D46" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="19"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="19"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
       <c r="G48" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="19"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
       <c r="G49" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="19"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
       <c r="G50" s="7" t="s">
         <v>115</v>
       </c>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="19"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
       <c r="G51" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
       <c r="G52" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="16" t="s">
         <v>93</v>
       </c>
       <c r="G53" s="8" t="s">
@@ -1929,162 +1977,162 @@
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
       <c r="G54" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
       <c r="G55" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
       <c r="D56" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
       <c r="G56" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
       <c r="D57" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
       <c r="G57" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
       <c r="D58" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
       <c r="G58" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="21"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
       <c r="D59" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
       <c r="G59" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
       <c r="D60" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
       <c r="G60" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
       <c r="D61" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
       <c r="G61" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="21"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
       <c r="D62" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
       <c r="G62" s="8" t="s">
         <v>117</v>
       </c>
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
       <c r="G63" s="8" t="s">
         <v>116</v>
       </c>
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="19" t="s">
         <v>65</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E64" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F64" s="18" t="s">
+      <c r="F64" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G64" s="7" t="s">
@@ -2092,110 +2140,122 @@
       </c>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
       <c r="G65" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="19"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19"/>
+      <c r="H65" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
       <c r="G66" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
+      <c r="H66" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
       <c r="D67" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
       <c r="G67" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H67" s="7"/>
+      <c r="H67" s="15" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
       <c r="G68" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
+      <c r="H68" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
       <c r="D69" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
       <c r="G69" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
+      <c r="H69" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
       <c r="G70" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H70" s="7"/>
+      <c r="H70" s="15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="16" t="s">
         <v>100</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="G71" s="14" t="s">
+      <c r="G71" s="16" t="s">
         <v>104</v>
       </c>
       <c r="H71" s="11" t="s">
@@ -2203,67 +2263,67 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
       <c r="D72" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="14" t="s">
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="16" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="21"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
+      <c r="A73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
       <c r="D73" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="15"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="18"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="14" t="s">
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
       <c r="H74" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="21"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
       <c r="H75" s="11" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="15"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="18"/>
       <c r="C76" s="12"/>
       <c r="D76" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
       <c r="H76" s="11" t="s">
         <v>138</v>
       </c>
@@ -2970,53 +3030,6 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="C64:C70"/>
-    <mergeCell ref="A64:A70"/>
-    <mergeCell ref="B43:B52"/>
-    <mergeCell ref="B64:B70"/>
-    <mergeCell ref="C43:C52"/>
-    <mergeCell ref="A43:A52"/>
-    <mergeCell ref="C53:C63"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="B53:B63"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="E35:E42"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="C35:C42"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="F64:F70"/>
-    <mergeCell ref="E43:E52"/>
-    <mergeCell ref="E64:E70"/>
-    <mergeCell ref="E53:E63"/>
-    <mergeCell ref="F53:F63"/>
-    <mergeCell ref="F43:F52"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="A13:A29"/>
-    <mergeCell ref="B13:B29"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C13:C29"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E71:E76"/>
-    <mergeCell ref="F71:F76"/>
-    <mergeCell ref="G71:G76"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="G26:G27"/>
@@ -3030,6 +3043,53 @@
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F3:F12"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="F71:F76"/>
+    <mergeCell ref="G71:G76"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C13:C29"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="A13:A29"/>
+    <mergeCell ref="B13:B29"/>
+    <mergeCell ref="F64:F70"/>
+    <mergeCell ref="E43:E52"/>
+    <mergeCell ref="E64:E70"/>
+    <mergeCell ref="E53:E63"/>
+    <mergeCell ref="F53:F63"/>
+    <mergeCell ref="F43:F52"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="E35:E42"/>
+    <mergeCell ref="F35:F42"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B43:B52"/>
+    <mergeCell ref="B64:B70"/>
+    <mergeCell ref="C43:C52"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="C53:C63"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="B53:B63"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="C64:C70"/>
+    <mergeCell ref="A64:A70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>